<commit_message>
Dashboard updates - 15/04/2024
</commit_message>
<xml_diff>
--- a/EFM_shiny.xlsx
+++ b/EFM_shiny.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7650" tabRatio="971" firstSheet="1" activeTab="5"/>
+    <workbookView windowWidth="20490" windowHeight="7650" tabRatio="971" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="contents" sheetId="2" r:id="rId1"/>
@@ -165,10 +165,10 @@
     <t>text = "App Last Launch", colour = "blue"</t>
   </si>
   <si>
-    <t>%&gt;% filter(!is.na(app_last_launch)) %&gt;% group_by(app_last_launch) %&gt;% summarise(frequency = n())</t>
-  </si>
-  <si>
-    <t>geom_line(aes(x = app_last_launch, y = frequency)) + geom_point(aes(x = app_last_launch, y = frequency)) + labs(x = "Date", y = "Frequency", title = "Frequency of Values by Date")</t>
+    <t>%&gt;% filter(!is.na(app_last_launch_month)) %&gt;% group_by(app_last_launch_month) %&gt;% summarise(frequency = n())</t>
+  </si>
+  <si>
+    <t>geom_line(aes(x = app_last_launch_month, y = frequency)) + geom_point(aes(x = app_last_launch_month, y = frequency)) + labs(x = "Date", y = "Frequency", title = "Frequency of Values by Date")</t>
   </si>
   <si>
     <t>text = "App Launch Count", colour = "blue"</t>
@@ -1502,8 +1502,8 @@
   <sheetPr/>
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="P17" sqref="P17"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="6"/>
@@ -1929,7 +1929,7 @@
   <sheetPr/>
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>

</xml_diff>